<commit_message>
added graphing on graph_per_genre function
</commit_message>
<xml_diff>
--- a/books_I_want_to_read.xlsx
+++ b/books_I_want_to_read.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abilashsivasith/Desktop/Repo/Book_Data_Display/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F75A54-061C-734A-8D8B-B6D61EA2BA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8804736D-ED3D-5C4B-977E-A8763FDECF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{979CF706-70E0-4F75-AA5B-8FEB5E99BE77}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="368">
   <si>
     <t>Tittle</t>
   </si>
@@ -2251,9 +2251,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2291,7 +2291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2397,7 +2397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2539,7 +2539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2549,8 +2549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B5247B-DC07-4C30-82C7-CA7E37F6266D}">
   <dimension ref="A1:H178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="125" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5599,7 +5599,9 @@
         <v>335</v>
       </c>
       <c r="C150" s="7"/>
-      <c r="D150" s="7"/>
+      <c r="D150" s="7" t="s">
+        <v>90</v>
+      </c>
       <c r="E150" s="7" t="s">
         <v>6</v>
       </c>
@@ -5795,7 +5797,9 @@
         <v>364</v>
       </c>
       <c r="C162" s="7"/>
-      <c r="D162" s="7"/>
+      <c r="D162" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="E162" s="7" t="s">
         <v>340</v>
       </c>

</xml_diff>